<commit_message>
completed test_plan_rectangle.xlsx file with all test cases
</commit_message>
<xml_diff>
--- a/tests/test_plan_rectangle.xlsx
+++ b/tests/test_plan_rectangle.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>#VALUE!</t>
   </si>
@@ -58,28 +58,67 @@
     <t>Attribute  set to input values.</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>color="red",                                                           length=5,                                                                width=6</t>
+  </si>
+  <si>
+    <t>Attributes set: _color="red",                   _length=5,                                                 -width=6</t>
+  </si>
+  <si>
     <t>Exception raised when color is blank</t>
   </si>
   <si>
+    <t>color=" ",                                                 length=5,                                                   width=6</t>
+  </si>
+  <si>
+    <t>ValueError: "Color cannot be blank."</t>
+  </si>
+  <si>
     <t>Exception raised when length is not an integer.</t>
   </si>
   <si>
+    <t>color="red",                                       length="five",                                          width=6</t>
+  </si>
+  <si>
+    <t>ValueError:"Length must be numeric."</t>
+  </si>
+  <si>
     <t>Exception raised when width is not an integer.</t>
   </si>
   <si>
+    <t>color="red",                                           length=5,                                           width="six"</t>
+  </si>
+  <si>
+    <t>ValueError: "Width must be numeric."</t>
+  </si>
+  <si>
     <t>__str__</t>
   </si>
   <si>
     <t>Returns string formatted appropriately</t>
   </si>
   <si>
+    <t>Valid instance</t>
+  </si>
+  <si>
+    <t>"The shape color is red.\nThis rectangle has four sides with the lengths of 5, 6, 5 and 6 centimeters."</t>
+  </si>
+  <si>
     <t>calculate_area</t>
   </si>
   <si>
     <t>Returns correct calculated value.</t>
   </si>
   <si>
+    <t xml:space="preserve">Correct area value(example, 12 for length=3, width=4) </t>
+  </si>
+  <si>
     <t>calculate_perimeter</t>
+  </si>
+  <si>
+    <t>Correct perimeter value(example, 14 for length=3, width=4)</t>
   </si>
   <si>
     <t>Add more rows as necessary</t>
@@ -865,7 +904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="72.75">
       <c r="A7" s="16"/>
       <c r="B7" s="17">
         <v>1</v>
@@ -876,9 +915,15 @@
       <c r="D7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="E7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="66.75">
       <c r="A8" s="16"/>
@@ -889,11 +934,17 @@
         <v>12</v>
       </c>
       <c r="D8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+      <c r="F8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="74.25">
       <c r="A9" s="16"/>
@@ -904,11 +955,17 @@
         <v>12</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="78.75">
       <c r="A10" s="16"/>
@@ -919,26 +976,38 @@
         <v>12</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="61.5" customFormat="1" s="21">
+        <v>23</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="91.5" customFormat="1" s="21">
       <c r="A11" s="22"/>
       <c r="B11" s="17">
         <v>5</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+        <v>27</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="63.75">
       <c r="A12" s="1"/>
@@ -946,14 +1015,20 @@
         <v>6</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+        <v>31</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="31.149999999999995">
       <c r="A13" s="1"/>
@@ -961,14 +1036,20 @@
         <v>7</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
+        <v>31</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="31.149999999999995" customFormat="1" s="21">
       <c r="A14" s="22"/>
@@ -1092,7 +1173,7 @@
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
       <c r="B25" s="24" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>

</xml_diff>